<commit_message>
added checkboxes to mark completed next to each row
</commit_message>
<xml_diff>
--- a/A2Rubric.xlsx
+++ b/A2Rubric.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stanton\Desktop\A2Group12\A2Group12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Downloads\RMIT Assignments\Assignment_2_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089FF801-46CE-4742-A368-A07E9377848E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" showSheetTabs="0" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -105,8 +106,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,6 +143,11 @@
       <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -231,6 +237,821 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>314325</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>428625</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>523875</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4707E24-023F-4018-81E9-3D75FC03A7E9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Completed</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>314325</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>428625</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>523875</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1026" name="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1026"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F87C46A-4ADF-4648-BF47-7DAD5B48B05E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Completed</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>314325</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>428625</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>523875</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1027" name="Check Box 3" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1027"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{238F7822-C93D-44DC-884E-7760362D0E04}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Completed</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>314325</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>428625</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>523875</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1028" name="Check Box 4" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1028"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B9A9A51-B6A5-49AF-88F6-DE5722B36A28}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Completed</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>314325</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>428625</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>523875</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1029"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36D0D1D1-05C6-45F2-B025-457C82A08D7A}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Completed</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>428625</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>419100</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1030"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D35A5C1-A918-499A-98E3-564B738FA389}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Completed</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>314325</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>428625</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>523875</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1031"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E05EE021-FACE-4E60-932B-878F391B24F3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Completed</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>314325</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>428625</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>523875</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1032"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{362248A6-F011-4CFC-B0A5-4CA2A16F1D90}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Completed</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>238125</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>209550</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>428625</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>419100</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1033" name="Check Box 9" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1033"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73EE3CBD-B566-430D-B2F3-6B8000885B3E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="18288" rIns="0" bIns="18288" anchor="ctr" upright="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l" rtl="0">
+                <a:defRPr sz="1000"/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-AU" sz="800" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Segoe UI"/>
+                  <a:cs typeface="Segoe UI"/>
+                </a:rPr>
+                <a:t>Completed</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -495,11 +1316,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,5 +1439,211 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1025" r:id="rId4" name="Check Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>314325</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>428625</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>523875</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1026" r:id="rId5" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>314325</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>428625</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>523875</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1027" r:id="rId6" name="Check Box 3">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>314325</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>428625</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>523875</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1028" r:id="rId7" name="Check Box 4">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>314325</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>428625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>523875</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1029" r:id="rId8" name="Check Box 5">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>314325</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>428625</xdr:colOff>
+                    <xdr:row>8</xdr:row>
+                    <xdr:rowOff>523875</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1030" r:id="rId9" name="Check Box 6">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>428625</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>419100</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1031" r:id="rId10" name="Check Box 7">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>314325</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>428625</xdr:colOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>523875</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1032" r:id="rId11" name="Check Box 8">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>314325</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>428625</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>523875</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1033" r:id="rId12" name="Check Box 9">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>2</xdr:col>
+                    <xdr:colOff>238125</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>209550</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>428625</xdr:colOff>
+                    <xdr:row>16</xdr:row>
+                    <xdr:rowOff>419100</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>